<commit_message>
feat: add DataHandler's property test; add GetGrade method test
</commit_message>
<xml_diff>
--- a/OnlineCoursesAnalyzerTests/Data/EducationalAchievmentDataWithSomeErrors.xlsx
+++ b/OnlineCoursesAnalyzerTests/Data/EducationalAchievmentDataWithSomeErrors.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="89">
   <si>
     <t>Student ID</t>
   </si>
@@ -159,9 +159,6 @@
     <t>honor</t>
   </si>
   <si>
-    <t>st000002@student.spbu.ru</t>
-  </si>
-  <si>
     <t>1.0</t>
   </si>
   <si>
@@ -265,6 +262,30 @@
   </si>
   <si>
     <t>unknown</t>
+  </si>
+  <si>
+    <t>st000006@student.spbu.ru</t>
+  </si>
+  <si>
+    <t>st000007@student.spbu.ru</t>
+  </si>
+  <si>
+    <t>st000008@student.spbu.ru</t>
+  </si>
+  <si>
+    <t>st000009@student.spbu.ru</t>
+  </si>
+  <si>
+    <t>st000006</t>
+  </si>
+  <si>
+    <t>st000007</t>
+  </si>
+  <si>
+    <t>st000008</t>
+  </si>
+  <si>
+    <t>st000009</t>
   </si>
 </sst>
 </file>
@@ -368,7 +389,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -392,6 +413,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -678,7 +702,7 @@
   <dimension ref="A1:AG17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -896,10 +920,10 @@
         <v>62349</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>37</v>
@@ -998,22 +1022,22 @@
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="10" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>38</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I4" s="10" t="s">
         <v>38</v>
@@ -1095,26 +1119,26 @@
       <c r="A5" s="8">
         <v>394310</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>44</v>
+      <c r="B5" s="15" t="s">
+        <v>53</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>38</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I5" s="10" t="s">
         <v>38</v>
@@ -1196,92 +1220,92 @@
       <c r="A6" s="4">
         <v>2692245</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>46</v>
+      <c r="B6" s="14" t="s">
+        <v>59</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="I6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="S6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="T6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="U6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="V6" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="I6" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="O6" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="P6" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q6" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="R6" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="S6" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="T6" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="U6" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="V6" s="6" t="s">
+      <c r="W6" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="X6" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA6" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="W6" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="X6" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y6" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z6" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA6" s="6" t="s">
+      <c r="AB6" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="AB6" s="6" t="s">
+      <c r="AC6" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="AC6" s="6" t="s">
+      <c r="AD6" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="AD6" s="6" t="s">
-        <v>53</v>
       </c>
       <c r="AE6" s="6" t="s">
         <v>42</v>
@@ -1332,23 +1356,23 @@
       <c r="A8" s="8">
         <v>2714096</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>54</v>
+      <c r="B8" s="15" t="s">
+        <v>81</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H8" s="12">
         <v>60</v>
@@ -1357,67 +1381,67 @@
         <v>38</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K8" s="10" t="s">
         <v>38</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M8" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="N8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="O8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="P8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="R8" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="N8" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="O8" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="P8" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q8" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="R8" s="10" t="s">
+      <c r="S8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="T8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="U8" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="S8" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="T8" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="U8" s="10" t="s">
-        <v>59</v>
-      </c>
       <c r="V8" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="W8" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="X8" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y8" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z8" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA8" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="W8" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="X8" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y8" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z8" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA8" s="10" t="s">
+      <c r="AB8" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="AB8" s="10" t="s">
+      <c r="AC8" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="AC8" s="10" t="s">
+      <c r="AD8" s="10" t="s">
         <v>52</v>
-      </c>
-      <c r="AD8" s="10" t="s">
-        <v>53</v>
       </c>
       <c r="AE8" s="10" t="s">
         <v>42</v>
@@ -1433,92 +1457,92 @@
       <c r="A9" s="8">
         <v>2714096</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>54</v>
+      <c r="B9" s="15" t="s">
+        <v>82</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G9" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="M9" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="H9" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="I9" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="J9" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="K9" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="L9" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="M9" s="10" t="s">
+      <c r="N9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="O9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="P9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="R9" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="N9" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="O9" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="P9" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q9" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="R9" s="10" t="s">
+      <c r="S9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="T9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="U9" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="S9" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="T9" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="U9" s="10" t="s">
-        <v>59</v>
-      </c>
       <c r="V9" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="W9" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="X9" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y9" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z9" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA9" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="W9" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="X9" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y9" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z9" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA9" s="10" t="s">
+      <c r="AB9" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="AB9" s="10" t="s">
+      <c r="AC9" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="AC9" s="10" t="s">
+      <c r="AD9" s="10" t="s">
         <v>52</v>
-      </c>
-      <c r="AD9" s="10" t="s">
-        <v>53</v>
       </c>
       <c r="AE9" s="10" t="s">
         <v>42</v>
@@ -1534,90 +1558,90 @@
       <c r="A10" s="4">
         <v>2714100</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>60</v>
+      <c r="B10" s="14" t="s">
+        <v>83</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H10" s="13">
         <v>75</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N10" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="O10" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="P10" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q10" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="R10" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="O10" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="P10" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q10" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="R10" s="6" t="s">
+      <c r="S10" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="T10" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="U10" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="S10" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="T10" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="U10" s="6" t="s">
-        <v>65</v>
-      </c>
       <c r="V10" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="W10" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="X10" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y10" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z10" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA10" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="W10" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="X10" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y10" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z10" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA10" s="6" t="s">
+      <c r="AB10" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="AB10" s="6" t="s">
+      <c r="AC10" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="AC10" s="6" t="s">
+      <c r="AD10" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="AD10" s="6" t="s">
-        <v>53</v>
       </c>
       <c r="AE10" s="6" t="s">
         <v>42</v>
@@ -1633,92 +1657,92 @@
       <c r="A11" s="4">
         <v>2714100</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>60</v>
+      <c r="B11" s="14" t="s">
+        <v>84</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H11" s="13">
         <v>75</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N11" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q11" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="R11" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="O11" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="P11" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q11" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="R11" s="6" t="s">
+      <c r="S11" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="T11" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="U11" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="S11" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="T11" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="U11" s="6" t="s">
-        <v>65</v>
-      </c>
       <c r="V11" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="W11" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="X11" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA11" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="W11" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="X11" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y11" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z11" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA11" s="6" t="s">
+      <c r="AB11" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="AB11" s="6" t="s">
+      <c r="AC11" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="AC11" s="6" t="s">
+      <c r="AD11" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="AD11" s="6" t="s">
-        <v>53</v>
       </c>
       <c r="AE11" s="6" t="s">
         <v>42</v>

</xml_diff>